<commit_message>
Added parsing for holes
</commit_message>
<xml_diff>
--- a/excel documents/course.xlsx
+++ b/excel documents/course.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\github\1dv503\database_assignment3\excel documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/775cb088da073b9b/Dokument/Knacka_kod/Phyton/1DV503/database_assignment3/excel documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFC2A40-CE26-4560-9BD4-BAC7A4244F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{EEFC2A40-CE26-4560-9BD4-BAC7A4244F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A990466F-4B56-4FE4-93D0-2EEE8112ABF4}"/>
   <bookViews>
-    <workbookView xWindow="17220" yWindow="6585" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5160" yWindow="840" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,10 @@
     <t>hole</t>
   </si>
   <si>
-    <t>almhults discgoldbana</t>
+    <t>Teleborgs discgolfbana</t>
   </si>
   <si>
-    <t>Teleborgs discgolfbana</t>
+    <t>almhults discgolfbana</t>
   </si>
 </sst>
 </file>
@@ -362,17 +362,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,9 +386,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -400,9 +400,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -414,9 +414,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -428,9 +428,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -442,9 +442,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -456,9 +456,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -470,9 +470,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -484,9 +484,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -498,9 +498,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -512,9 +512,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -526,9 +526,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -540,9 +540,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -554,9 +554,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -568,9 +568,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -582,9 +582,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -596,9 +596,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>7</v>
@@ -610,9 +610,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -624,9 +624,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19">
         <v>9</v>
@@ -638,9 +638,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -652,9 +652,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21">
         <v>11</v>
@@ -666,9 +666,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B22">
         <v>12</v>
@@ -680,9 +680,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B23">
         <v>13</v>
@@ -694,9 +694,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B24">
         <v>14</v>
@@ -708,9 +708,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B25">
         <v>15</v>
@@ -722,9 +722,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B26">
         <v>16</v>
@@ -736,9 +736,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27">
         <v>17</v>
@@ -750,9 +750,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B28">
         <v>18</v>

</xml_diff>